<commit_message>
CDR-2102_1357 summer tour changes done
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\misha\workspace\Revision5Day1POMCI\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE10428-C7BA-4FA1-8D09-C7ECEA7B6FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D76658C-4C10-426D-A0D7-5D77A6CB9A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="winterToursTest" sheetId="1" r:id="rId1"/>
+    <sheet name="summerToursTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -49,6 +50,18 @@
   </si>
   <si>
     <t>Hi This is Khaleefullah from Chennai</t>
+  </si>
+  <si>
+    <t>Amanullah Akbar Ali</t>
+  </si>
+  <si>
+    <t>amanullah.a@gmail.com</t>
+  </si>
+  <si>
+    <t>9943357865</t>
+  </si>
+  <si>
+    <t>Hi This is Amanullah from Erode</t>
   </si>
 </sst>
 </file>
@@ -396,7 +409,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -442,4 +457,57 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4155B9A7-45EB-4F82-B3E1-922AD6B0CC34}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{4B8E065A-986C-4FE1-8CA3-416DF7EAF8A0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>